<commit_message>
Optimisation avec 3 BufferedReader et lecture sequentielle du fichier
</commit_message>
<xml_diff>
--- a/Tests_Unitaires/dataset_20.xlsx
+++ b/Tests_Unitaires/dataset_20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\OPTION1\HPP\Projet_Coronavirus\HPP_Coronavirus_Project\Tests_Unitaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED67F7D6-56A3-4550-B25D-1AEE255A9B63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACB7624-02D2-4B97-865A-F20CAB1E87F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Output</t>
   </si>
@@ -148,7 +148,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -196,7 +196,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -482,7 +482,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Ajout du premier test unitaire traitant entièrement le fichier 20
</commit_message>
<xml_diff>
--- a/Tests_Unitaires/dataset_20.xlsx
+++ b/Tests_Unitaires/dataset_20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Documents\Temporaire\FISE2\OPTION1\HPP\Projet_Coronavirus\HPP_Coronavirus_Project\Tests_Unitaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACB7624-02D2-4B97-865A-F20CAB1E87F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8F74D8-BA01-4B6E-B7BA-08D2D7D6B4D6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11000" yWindow="770" windowWidth="14130" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -45,79 +45,79 @@
     <t>Différence de jours</t>
   </si>
   <si>
-    <t>Spain, 0, 10</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>1 jour =</t>
   </si>
   <si>
-    <t>Italy, 1, 10</t>
-  </si>
-  <si>
-    <t>Spain, 2, 10</t>
-  </si>
-  <si>
-    <t>Spain, 3, 10</t>
-  </si>
-  <si>
-    <t>France, 4, 10; Spain, 3, 4</t>
-  </si>
-  <si>
-    <t>Italy, 6, 10; France, 5, 4</t>
-  </si>
-  <si>
-    <t>Spain, 7, 10; Italy, 6, 4</t>
-  </si>
-  <si>
     <t>Cumul 2 itérations</t>
   </si>
   <si>
     <t>Cumul 3 itérations</t>
   </si>
   <si>
-    <t>France, 5, 10; France, 4, 4</t>
-  </si>
-  <si>
-    <t>Spain, 7, 10; Spain 8, 10</t>
-  </si>
-  <si>
-    <t>Spain, 8, 10; France, 9, 10; Spain, 7, 4</t>
-  </si>
-  <si>
-    <t>France, 9, 10; Italy, 10, 10; Spain, 8, 4</t>
-  </si>
-  <si>
-    <t>Italy 10, 10; Spain, 11, 10; France, 9, 4</t>
-  </si>
-  <si>
-    <t>Spain, 11, 10; Italy, 12, 10; Italy 10, 4</t>
-  </si>
-  <si>
-    <t>Italy, 12, 10; France, 13, 10; Spain, 11, 4</t>
-  </si>
-  <si>
-    <t>France, 13, 10; France, 14, 10; Spain, 11, 4; Italy, 12, 4</t>
-  </si>
-  <si>
     <t>Cumul 4 itérations</t>
   </si>
   <si>
-    <t>France, 14, 10; Italy, 15, 10; France, 13, 4; Italy, 12, 4</t>
-  </si>
-  <si>
-    <t>Italy, 15, 10; Spain, 16, 10; France, 13, 4; France, 14, 4</t>
-  </si>
-  <si>
-    <t>Italy, 15, 10; Spain, 16, 10; Italy, 17, 10; France, 13, 4</t>
-  </si>
-  <si>
-    <t>Spain, 16, 10; Italy, 17, 10; Italy, 18, 10; France, 13, 4: Italy, 15, 4</t>
-  </si>
-  <si>
     <t>Cumul 5 itérations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France, 14, 10; Italy, 15, 10; Italy, 12, 4; France, 13, 4; </t>
+  </si>
+  <si>
+    <t>Spain, 0, 10;</t>
+  </si>
+  <si>
+    <t>Italy, 1, 10;</t>
+  </si>
+  <si>
+    <t>Spain, 2, 10;</t>
+  </si>
+  <si>
+    <t>Spain, 3, 10;</t>
+  </si>
+  <si>
+    <t>France, 4, 10; Spain, 3, 4;</t>
+  </si>
+  <si>
+    <t>France, 5, 10; France, 4, 4;</t>
+  </si>
+  <si>
+    <t>Italy, 6, 10; France, 5, 4;</t>
+  </si>
+  <si>
+    <t>Spain, 7, 10; Italy, 6, 4;</t>
+  </si>
+  <si>
+    <t>Spain, 7, 10; Spain 8, 10;</t>
+  </si>
+  <si>
+    <t>Spain, 8, 10; France, 9, 10; Spain, 7, 4;</t>
+  </si>
+  <si>
+    <t>France, 9, 10; Italy, 10, 10; Spain, 8, 4;</t>
+  </si>
+  <si>
+    <t>Italy 10, 10; Spain, 11, 10; France, 9, 4;</t>
+  </si>
+  <si>
+    <t>Spain, 11, 10; Italy, 12, 10; Italy 10, 4;</t>
+  </si>
+  <si>
+    <t>Italy, 12, 10; France, 13, 10; Spain, 11, 4;</t>
+  </si>
+  <si>
+    <t>France, 13, 10; France, 14, 10; Spain, 11, 4; Italy, 12, 4;</t>
+  </si>
+  <si>
+    <t>Italy, 15, 10; Spain, 16, 10; France, 13, 4; France, 14, 4;</t>
+  </si>
+  <si>
+    <t>Italy, 15, 10; Spain, 16, 10; Italy, 17, 10; France, 13, 4;</t>
+  </si>
+  <si>
+    <t>Spain, 16, 10; Italy, 17, 10; Italy, 18, 10; France, 13, 4: Italy, 15, 4;</t>
   </si>
   <si>
     <r>
@@ -139,7 +139,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Italy, 15, 4; Spain, 16, 4</t>
+      <t xml:space="preserve"> Italy, 15, 4; Spain, 16, 4;</t>
     </r>
   </si>
 </sst>
@@ -481,8 +481,8 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,19 +505,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1">
         <v>86400</v>
@@ -525,18 +525,18 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1573945200</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1577483620</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1579553464</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1581022041</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>1582161158</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>1583091884</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>1583878802</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>1584560462</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1585161728</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>1585699579</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>1586186124</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>1586630305</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>1587038912</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>1587417223</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>1587769422</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>1588098882</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>1588408363</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>1588700149</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>1588976154</v>

</xml_diff>